<commit_message>
Adicionado alguns comentários no código
</commit_message>
<xml_diff>
--- a/data/dados_acch.xlsx
+++ b/data/dados_acch.xlsx
@@ -5,8 +5,8 @@
   <sheets>
     <sheet state="visible" name="dados_de_barra" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="dados_de_linha" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="dados_de_geradores" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Página4" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="dados_dos_geradores" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="dados_dos_transformadores" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -439,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -471,6 +471,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3557,8 +3560,14 @@
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+    </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
@@ -3570,24 +3579,33 @@
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+    </row>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -4572,49 +4590,49 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="14" t="s">
         <v>78</v>
       </c>
     </row>
@@ -7440,7 +7458,7 @@
       <c r="D35" s="6">
         <v>3.0</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="15" t="s">
         <v>94</v>
       </c>
       <c r="F35" s="6">

</xml_diff>